<commit_message>
feat: update BagItem xlsx
</commit_message>
<xml_diff>
--- a/Excels/BagItem_背包物品表.xlsx
+++ b/Excels/BagItem_背包物品表.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>int</t>
   </si>
@@ -27,7 +27,7 @@
     <t>name</t>
   </si>
   <si>
-    <t>series</t>
+    <t>desc</t>
   </si>
   <si>
     <t>stackCount</t>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>测试用物品</t>
+  </si>
+  <si>
+    <t>DragonFruit</t>
+  </si>
+  <si>
+    <t>火龙果</t>
   </si>
 </sst>
 </file>
@@ -650,7 +656,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -664,19 +670,16 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf fontId="21" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf fontId="22" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -778,13 +781,13 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="double">
           <color theme="4"/>
         </top>
-        <bottom/>
-        <diagonal/>
+        <bottom style="none"/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -804,7 +807,7 @@
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
         <horizontal style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </horizontal>
@@ -831,13 +834,13 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -846,15 +849,15 @@
         <color theme="1"/>
       </font>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="thin">
           <color theme="4"/>
         </top>
         <bottom style="thin">
           <color theme="4"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -869,13 +872,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -889,13 +892,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -906,13 +909,13 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
-        <top/>
+        <left style="none"/>
+        <right style="none"/>
+        <top style="none"/>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
     <dxf>
@@ -938,15 +941,15 @@
         </patternFill>
       </fill>
       <border>
-        <left/>
-        <right/>
+        <left style="none"/>
+        <right style="none"/>
         <top style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </top>
         <bottom style="thin">
           <color theme="4" tint="0.39997558519241899"/>
         </bottom>
-        <diagonal/>
+        <diagonal style="none"/>
       </border>
     </dxf>
   </dxfs>
@@ -1572,7 +1575,7 @@
       <c r="C3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -1603,7 +1606,7 @@
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
-      <c r="I4" s="6"/>
+      <c r="I4" s="5"/>
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
       <c r="L4" s="1"/>
@@ -1615,26 +1618,26 @@
       <c r="R4" s="1"/>
     </row>
     <row r="5" s="1" customFormat="1" ht="30">
-      <c r="A5" s="6">
+      <c r="A5" s="5">
         <v>1</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="1">
         <v>64</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="7">
         <v>222920</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="8"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="6"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
@@ -1645,16 +1648,26 @@
       <c r="R5" s="1"/>
     </row>
     <row r="6" s="1" customFormat="1" ht="30">
-      <c r="A6" s="1"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="9"/>
+      <c r="A6" s="1">
+        <v>2</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="1">
+        <v>999</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="8"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
       <c r="M6" s="1"/>
@@ -1665,16 +1678,16 @@
       <c r="R6" s="1"/>
     </row>
     <row r="7" s="1" customFormat="1" ht="30">
-      <c r="A7" s="6"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="9"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="1"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="8"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="6"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
       <c r="M7" s="1"/>
@@ -1685,16 +1698,16 @@
       <c r="R7" s="1"/>
     </row>
     <row r="8" s="1" customFormat="1" ht="30">
-      <c r="A8" s="6"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="9"/>
+      <c r="E8" s="7"/>
       <c r="F8" s="1"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="8"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="6"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
       <c r="M8" s="1"/>
@@ -1705,16 +1718,16 @@
       <c r="R8" s="1"/>
     </row>
     <row r="9" s="1" customFormat="1" ht="30">
-      <c r="A9" s="6"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="9"/>
+      <c r="E9" s="7"/>
       <c r="F9" s="1"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="8"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="6"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
@@ -1725,16 +1738,16 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" s="1" customFormat="1" ht="30">
-      <c r="A10" s="6"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="9"/>
+      <c r="E10" s="7"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="8"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="6"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
@@ -1745,13 +1758,13 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" s="1" customFormat="1">
-      <c r="A11" s="8"/>
+      <c r="A11" s="6"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="8"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="6"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1762,12 +1775,12 @@
       <c r="R11" s="1"/>
     </row>
     <row r="12" s="1" customFormat="1">
-      <c r="A12" s="8"/>
+      <c r="A12" s="6"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="8"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="6"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
       <c r="M12" s="1"/>
@@ -1778,156 +1791,156 @@
       <c r="R12" s="1"/>
     </row>
     <row r="13" s="1" customFormat="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
-      <c r="C13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
+      <c r="E13" s="7"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="7"/>
+      <c r="L13" s="5"/>
       <c r="M13" s="1"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
-      <c r="Q13" s="9"/>
-      <c r="R13" s="9"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
     </row>
     <row r="14" s="1" customFormat="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="9"/>
+      <c r="A14" s="6"/>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="8"/>
-      <c r="M14" s="8"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="9"/>
-      <c r="P14" s="9"/>
-      <c r="Q14" s="9"/>
-      <c r="R14" s="9"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
     </row>
     <row r="15" s="1" customFormat="1">
-      <c r="A15" s="8"/>
+      <c r="A15" s="6"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="P15" s="9"/>
-      <c r="Q15" s="9"/>
-      <c r="R15" s="9"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="7"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
     </row>
     <row r="16" s="1" customFormat="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="6"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="8"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="P16" s="9"/>
-      <c r="Q16" s="9"/>
-      <c r="R16" s="9"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
     </row>
     <row r="17" s="1" customFormat="1">
-      <c r="A17" s="8"/>
+      <c r="A17" s="6"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="8"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="9"/>
-      <c r="R17" s="9"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
     </row>
     <row r="18" s="1" customFormat="1">
-      <c r="A18" s="8"/>
+      <c r="A18" s="6"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="9"/>
-      <c r="L18" s="6"/>
-      <c r="M18" s="8"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="P18" s="9"/>
-      <c r="Q18" s="9"/>
-      <c r="R18" s="9"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="5"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
     </row>
     <row r="19" s="1" customFormat="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="9"/>
-      <c r="C19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
+      <c r="A19" s="6"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="9"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="8"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="9"/>
-      <c r="P19" s="9"/>
-      <c r="Q19" s="9"/>
-      <c r="R19" s="9"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
     </row>
     <row r="20" s="1" customFormat="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="9"/>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
+      <c r="A20" s="6"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="9"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="8"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="9"/>
-      <c r="P20" s="9"/>
-      <c r="Q20" s="9"/>
-      <c r="R20" s="9"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="6"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="6"/>
+      <c r="M20" s="6"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
     </row>
     <row r="21" s="1" customFormat="1">
-      <c r="A21" s="8"/>
+      <c r="A21" s="6"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="8"/>
+      <c r="J21" s="6"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
@@ -1938,12 +1951,12 @@
       <c r="R21" s="1"/>
     </row>
     <row r="22" s="1" customFormat="1">
-      <c r="A22" s="8"/>
+      <c r="A22" s="6"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="8"/>
+      <c r="J22" s="6"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
@@ -1954,12 +1967,12 @@
       <c r="R22" s="1"/>
     </row>
     <row r="23" s="1" customFormat="1">
-      <c r="A23" s="8"/>
+      <c r="A23" s="6"/>
       <c r="F23" s="1"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="1"/>
-      <c r="J23" s="8"/>
+      <c r="J23" s="6"/>
       <c r="K23" s="1"/>
       <c r="L23" s="1"/>
       <c r="M23" s="1"/>
@@ -1970,12 +1983,12 @@
       <c r="R23" s="1"/>
     </row>
     <row r="24" s="1" customFormat="1">
-      <c r="A24" s="8"/>
+      <c r="A24" s="6"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="1"/>
-      <c r="J24" s="8"/>
+      <c r="J24" s="6"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
       <c r="M24" s="1"/>
@@ -1986,12 +1999,12 @@
       <c r="R24" s="1"/>
     </row>
     <row r="25" s="1" customFormat="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="6"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="5"/>
       <c r="I25" s="1"/>
-      <c r="J25" s="8"/>
+      <c r="J25" s="6"/>
       <c r="K25" s="1"/>
       <c r="L25" s="1"/>
       <c r="M25" s="1"/>
@@ -2002,16 +2015,16 @@
       <c r="R25" s="1"/>
     </row>
     <row r="26" s="1" customFormat="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="9"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="9"/>
-      <c r="E26" s="9"/>
+      <c r="A26" s="6"/>
+      <c r="B26" s="7"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="5"/>
       <c r="I26" s="1"/>
-      <c r="J26" s="8"/>
+      <c r="J26" s="6"/>
       <c r="K26" s="1"/>
       <c r="L26" s="1"/>
       <c r="M26" s="1"/>
@@ -2022,16 +2035,16 @@
       <c r="R26" s="1"/>
     </row>
     <row r="27" s="1" customFormat="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
+      <c r="A27" s="6"/>
+      <c r="B27" s="7"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="5"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="8"/>
+      <c r="J27" s="6"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
       <c r="M27" s="1"/>
@@ -2042,12 +2055,12 @@
       <c r="R27" s="1"/>
     </row>
     <row r="28" s="1" customFormat="1">
-      <c r="A28" s="8"/>
+      <c r="A28" s="6"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="5"/>
       <c r="I28" s="1"/>
-      <c r="J28" s="8"/>
+      <c r="J28" s="6"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
       <c r="M28" s="1"/>
@@ -2058,12 +2071,12 @@
       <c r="R28" s="1"/>
     </row>
     <row r="29" s="1" customFormat="1">
-      <c r="A29" s="8"/>
+      <c r="A29" s="6"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="5"/>
       <c r="I29" s="1"/>
-      <c r="J29" s="8"/>
+      <c r="J29" s="6"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
@@ -2074,12 +2087,12 @@
       <c r="R29" s="1"/>
     </row>
     <row r="30" s="1" customFormat="1">
-      <c r="A30" s="8"/>
+      <c r="A30" s="6"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="5"/>
       <c r="I30" s="1"/>
-      <c r="J30" s="8"/>
+      <c r="J30" s="6"/>
       <c r="K30" s="1"/>
       <c r="L30" s="1"/>
       <c r="M30" s="1"/>
@@ -2090,12 +2103,12 @@
       <c r="R30" s="1"/>
     </row>
     <row r="31" s="1" customFormat="1">
-      <c r="A31" s="8"/>
+      <c r="A31" s="6"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="5"/>
       <c r="I31" s="1"/>
-      <c r="J31" s="8"/>
+      <c r="J31" s="6"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -2106,12 +2119,12 @@
       <c r="R31" s="1"/>
     </row>
     <row r="32" s="1" customFormat="1">
-      <c r="A32" s="8"/>
+      <c r="A32" s="6"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="5"/>
       <c r="I32" s="1"/>
-      <c r="J32" s="8"/>
+      <c r="J32" s="6"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
       <c r="M32" s="1"/>
@@ -2122,12 +2135,12 @@
       <c r="R32" s="1"/>
     </row>
     <row r="33" s="1" customFormat="1">
-      <c r="A33" s="8"/>
+      <c r="A33" s="6"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="5"/>
       <c r="I33" s="1"/>
-      <c r="J33" s="8"/>
+      <c r="J33" s="6"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
@@ -2138,12 +2151,12 @@
       <c r="R33" s="1"/>
     </row>
     <row r="34" s="1" customFormat="1">
-      <c r="A34" s="8"/>
+      <c r="A34" s="6"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="5"/>
       <c r="I34" s="1"/>
-      <c r="J34" s="8"/>
+      <c r="J34" s="6"/>
       <c r="K34" s="1"/>
       <c r="L34" s="1"/>
       <c r="M34" s="1"/>
@@ -2154,12 +2167,12 @@
       <c r="R34" s="1"/>
     </row>
     <row r="35" s="1" customFormat="1">
-      <c r="A35" s="8"/>
+      <c r="A35" s="6"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="5"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="8"/>
+      <c r="J35" s="6"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
       <c r="M35" s="1"/>
@@ -2170,10 +2183,10 @@
       <c r="R35" s="1"/>
     </row>
     <row r="36" s="1" customFormat="1">
-      <c r="A36" s="8"/>
+      <c r="A36" s="6"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="5"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
@@ -2186,10 +2199,10 @@
       <c r="R36" s="1"/>
     </row>
     <row r="37" s="1" customFormat="1">
-      <c r="A37" s="8"/>
+      <c r="A37" s="6"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="5"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
@@ -2202,10 +2215,10 @@
       <c r="R37" s="1"/>
     </row>
     <row r="38" s="1" customFormat="1">
-      <c r="A38" s="8"/>
+      <c r="A38" s="6"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="8"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
@@ -2218,10 +2231,10 @@
       <c r="R38" s="1"/>
     </row>
     <row r="39" s="1" customFormat="1">
-      <c r="A39" s="8"/>
+      <c r="A39" s="6"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="8"/>
-      <c r="H39" s="8"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
@@ -2234,10 +2247,10 @@
       <c r="R39" s="1"/>
     </row>
     <row r="40" s="1" customFormat="1">
-      <c r="A40" s="8"/>
+      <c r="A40" s="6"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="8"/>
-      <c r="H40" s="8"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -2250,10 +2263,10 @@
       <c r="R40" s="1"/>
     </row>
     <row r="41" s="1" customFormat="1">
-      <c r="A41" s="8"/>
+      <c r="A41" s="6"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="8"/>
-      <c r="H41" s="8"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
@@ -2266,10 +2279,10 @@
       <c r="R41" s="1"/>
     </row>
     <row r="42" s="1" customFormat="1">
-      <c r="A42" s="8"/>
+      <c r="A42" s="6"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="8"/>
-      <c r="H42" s="8"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
@@ -2282,10 +2295,10 @@
       <c r="R42" s="1"/>
     </row>
     <row r="43" s="1" customFormat="1">
-      <c r="A43" s="8"/>
+      <c r="A43" s="6"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -2298,10 +2311,10 @@
       <c r="R43" s="1"/>
     </row>
     <row r="44" s="1" customFormat="1">
-      <c r="A44" s="8"/>
+      <c r="A44" s="6"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="8"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>

</xml_diff>

<commit_message>
feat: update Area configs
更新区域表，龙表，个性龙表
</commit_message>
<xml_diff>
--- a/Excels/BagItem_背包物品表.xlsx
+++ b/Excels/BagItem_背包物品表.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MetaApp\Editor_Win64\MetaWorldSaved\Saved\MetaWorld\Project\Edit\DragonVerse\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E3BA4C6-38E5-48BE-BB02-5E402621C191}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DCE7089-6FE8-4B39-BCC7-0C6651C6D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="3165" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="27">
   <si>
     <t>int</t>
   </si>
@@ -91,16 +91,18 @@
     <t>DragonName00001</t>
   </si>
   <si>
+    <t>TestBagItemDesc0001</t>
+  </si>
+  <si>
     <t>DragonName00002</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>DragonName00003</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>DragonName00004</t>
-  </si>
-  <si>
-    <t>TestBagItemDesc0001</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -632,7 +634,7 @@
   <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="16.5" x14ac:dyDescent="0.35"/>
@@ -822,7 +824,7 @@
         <v>22</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D9" s="7">
         <v>108377</v>
@@ -840,10 +842,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D10" s="7">
         <v>108377</v>
@@ -860,11 +862,11 @@
       <c r="A11" s="5">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>24</v>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D11" s="7">
         <v>108377</v>
@@ -881,11 +883,11 @@
       <c r="A12" s="1">
         <v>7</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>25</v>
+      <c r="B12" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="D12" s="7">
         <v>108377</v>
@@ -899,10 +901,21 @@
       <c r="I12" s="6"/>
     </row>
     <row r="13" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="6"/>
-      <c r="B13" s="7"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="7"/>
+      <c r="A13" s="1">
+        <v>8</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E13" s="1">
+        <v>1</v>
+      </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
@@ -916,10 +929,21 @@
       <c r="Q13" s="7"/>
     </row>
     <row r="14" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
+      <c r="A14" s="1">
+        <v>9</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1</v>
+      </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -934,7 +958,21 @@
       <c r="Q14" s="7"/>
     </row>
     <row r="15" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+      <c r="A15" s="5">
+        <v>10</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E15" s="1">
+        <v>1</v>
+      </c>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -949,7 +987,21 @@
       <c r="Q15" s="7"/>
     </row>
     <row r="16" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="6"/>
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -964,7 +1016,21 @@
       <c r="Q16" s="7"/>
     </row>
     <row r="17" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="6"/>
+      <c r="A17" s="1">
+        <v>12</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
       <c r="H17" s="5"/>
@@ -979,7 +1045,21 @@
       <c r="Q17" s="7"/>
     </row>
     <row r="18" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+      <c r="A18" s="1">
+        <v>13</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -994,10 +1074,21 @@
       <c r="Q18" s="7"/>
     </row>
     <row r="19" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="6"/>
-      <c r="B19" s="7"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="7"/>
+      <c r="A19" s="1">
+        <v>14</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
@@ -1012,10 +1103,21 @@
       <c r="Q19" s="7"/>
     </row>
     <row r="20" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="6"/>
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
+      <c r="A20" s="5">
+        <v>15</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1030,55 +1132,161 @@
       <c r="Q20" s="7"/>
     </row>
     <row r="21" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
+      <c r="A21" s="5">
+        <v>16</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="I21" s="6"/>
     </row>
     <row r="22" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
+      <c r="A22" s="1">
+        <v>17</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
       <c r="I22" s="6"/>
     </row>
     <row r="23" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+      <c r="A23" s="1">
+        <v>18</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1</v>
+      </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
       <c r="I23" s="6"/>
     </row>
     <row r="24" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+      <c r="A24" s="1">
+        <v>19</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
       <c r="I24" s="6"/>
     </row>
     <row r="25" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+      <c r="A25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
       <c r="F25" s="6"/>
       <c r="G25" s="5"/>
       <c r="I25" s="6"/>
     </row>
     <row r="26" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="6"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="A26" s="5">
+        <v>21</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E26" s="1">
+        <v>1</v>
+      </c>
       <c r="F26" s="6"/>
       <c r="G26" s="5"/>
       <c r="I26" s="6"/>
     </row>
     <row r="27" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="6"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="A27" s="1">
+        <v>22</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
       <c r="F27" s="6"/>
       <c r="G27" s="5"/>
       <c r="I27" s="6"/>
     </row>
     <row r="28" spans="1:17" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+      <c r="A28" s="1">
+        <v>23</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D28" s="7">
+        <v>108377</v>
+      </c>
+      <c r="E28" s="1">
+        <v>1</v>
+      </c>
       <c r="F28" s="6"/>
       <c r="G28" s="5"/>
       <c r="I28" s="6"/>

</xml_diff>